<commit_message>
s.c. cpmc 1.7 for coupled pBCS
</commit_message>
<xml_diff>
--- a/Fortran code/Fortran_bcs_pin_ettore/Record/record 8-27-2018.xlsx
+++ b/Fortran code/Fortran_bcs_pin_ettore/Record/record 8-27-2018.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1BAB0FEF-FC8B-4AE8-A04E-BD19D2307AFD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA15B847-94C0-4077-ADB9-14FFAE61B9A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t xml:space="preserve">Energy for t' models </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -88,6 +88,29 @@
   </si>
   <si>
     <t>CPMC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>44 u=4 6u6nPBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>44 u=4 7u7nPBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>44 u=4 8u8nPBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>t'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t' model</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -421,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -434,12 +457,12 @@
     <col min="4" max="4" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -462,7 +485,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -485,7 +508,7 @@
         <v>3.3628320769585884E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0.4</v>
       </c>
@@ -505,7 +528,7 @@
         <v>2.4561851595811972E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1.1000000000000001</v>
       </c>
@@ -525,7 +548,7 @@
         <v>2.2775266716798484E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>1.2</v>
       </c>
@@ -545,7 +568,7 @@
         <v>2.569795056995005E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1.5</v>
       </c>
@@ -565,7 +588,7 @@
         <v>1.8137351379660917E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -588,7 +611,7 @@
         <v>1.17480094120446E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>0.3</v>
       </c>
@@ -608,7 +631,7 @@
         <v>9.0202967341290654E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>0.35</v>
       </c>
@@ -628,7 +651,7 @@
         <v>9.3400028560467162E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>1.1499999999999999</v>
       </c>
@@ -648,7 +671,7 @@
         <v>9.0461747335535327E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>1.2</v>
       </c>
@@ -668,7 +691,7 @@
         <v>8.0411400227519657E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>1.5</v>
       </c>
@@ -686,6 +709,159 @@
       </c>
       <c r="G14">
         <v>7.57203645269255E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>0.2</v>
+      </c>
+      <c r="D17">
+        <v>-19.223496000000001</v>
+      </c>
+      <c r="E17">
+        <v>7.6816200000000001E-3</v>
+      </c>
+      <c r="F17">
+        <v>-19.189156195781042</v>
+      </c>
+      <c r="G17">
+        <v>5.320384503046051E-3</v>
+      </c>
+      <c r="H17">
+        <v>-19.181403599999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>-0.2</v>
+      </c>
+      <c r="D18">
+        <v>-17.716363510000001</v>
+      </c>
+      <c r="E18">
+        <v>4.99871E-3</v>
+      </c>
+      <c r="F18">
+        <v>-17.624560958986869</v>
+      </c>
+      <c r="G18">
+        <v>5.5370825400400435E-3</v>
+      </c>
+      <c r="H18">
+        <v>-17.761400026</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>0.2</v>
+      </c>
+      <c r="D20">
+        <v>-17.092968259999999</v>
+      </c>
+      <c r="E20">
+        <v>7.1702099999999998E-3</v>
+      </c>
+      <c r="F20">
+        <v>-16.773421572037179</v>
+      </c>
+      <c r="G20">
+        <v>8.1332819481685827E-3</v>
+      </c>
+      <c r="H20">
+        <v>-17.182938</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>-0.2</v>
+      </c>
+      <c r="D21">
+        <v>-16.414027180000001</v>
+      </c>
+      <c r="E21">
+        <v>5.6526299999999996E-3</v>
+      </c>
+      <c r="F21">
+        <v>-16.400135748483894</v>
+      </c>
+      <c r="G21">
+        <v>5.8861681275161892E-3</v>
+      </c>
+      <c r="H21">
+        <v>-16.410562599999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0.2</v>
+      </c>
+      <c r="D23">
+        <v>-13.503651550000001</v>
+      </c>
+      <c r="E23">
+        <v>1.403358E-2</v>
+      </c>
+      <c r="F23">
+        <v>-13.237823021738489</v>
+      </c>
+      <c r="G23">
+        <f>STDEV(F23:F43)/SQRT(20)</f>
+        <v>1.2260031653720184E-3</v>
+      </c>
+      <c r="H23">
+        <v>-13.627869</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>-0.2</v>
+      </c>
+      <c r="D24">
+        <v>-13.49667562</v>
+      </c>
+      <c r="E24">
+        <v>8.9199699999999993E-3</v>
+      </c>
+      <c r="F24">
+        <v>-13.245576946580792</v>
+      </c>
+      <c r="G24">
+        <v>8.2268898269285476E-3</v>
+      </c>
+      <c r="H24">
+        <v>-13.627869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>